<commit_message>
Cleaned up single-period unit chop, moved line chef to explicit column args.
</commit_message>
<xml_diff>
--- a/blackbird_engine/core/books/m10.xlsx
+++ b/blackbird_engine/core/books/m10.xlsx
@@ -1,24 +1,136 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Scenarios" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Timeline" sheetId="3" r:id="rId3"/>
-    <s:sheet name="wal-mart" sheetId="4" r:id="rId4"/>
-    <s:sheet name="existing 9" sheetId="5" r:id="rId5"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\blackbird\Engine\mechanics\spread_em\blackbird_engine\core\books\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13635" activeTab="4"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenarios" sheetId="2" r:id="rId2"/>
+    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
+    <sheet name="wal-mart" sheetId="4" r:id="rId4"/>
+    <sheet name="existing 9" sheetId="5" r:id="rId5"/>
+  </sheets>
+  <calcPr calcId="152511"/>
+</workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ilya</author>
+  </authors>
+  <commentList>
+    <comment ref="A23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ilya:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+These top-level drivers should still be indented
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ilya:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Should bold the summary lines and should only use "total" when the line has details</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ilya:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Need to fix these blank rows</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ilya:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ideally, blank items should get a 0 in the master and a link </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>annual_inflation</t>
   </si>
@@ -179,22 +291,48 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -210,17 +348,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -508,2281 +654,2258 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
         <f>E1</f>
-        <v/>
-      </c>
-      <c r="E1" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>0.03</v>
+      </c>
+      <c r="E1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
         <f>E2</f>
-        <v/>
-      </c>
-      <c r="E2" t="n">
-        <v>8080</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>8080</v>
+      </c>
+      <c r="E2">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
         <f>E3</f>
-        <v/>
-      </c>
-      <c r="E3" t="n">
+        <v>453.2</v>
+      </c>
+      <c r="E3">
         <v>453.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AO6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:41">
-      <c r="E3" s="1" t="n">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
         <v>42185</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="1">
         <v>42216</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="1">
         <v>42247</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>42277</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="1">
         <v>42308</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="1">
         <v>42338</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="1">
         <v>42369</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="1">
         <v>42400</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="1">
         <v>42429</v>
       </c>
-      <c r="N3" s="1" t="n">
+      <c r="N3" s="1">
         <v>42460</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="1">
         <v>42490</v>
       </c>
-      <c r="P3" s="1" t="n">
+      <c r="P3" s="1">
         <v>42521</v>
       </c>
-      <c r="Q3" s="1" t="n">
+      <c r="Q3" s="1">
         <v>42551</v>
       </c>
-      <c r="R3" s="1" t="n">
+      <c r="R3" s="1">
         <v>42582</v>
       </c>
-      <c r="S3" s="1" t="n">
+      <c r="S3" s="1">
         <v>42613</v>
       </c>
-      <c r="T3" s="1" t="n">
+      <c r="T3" s="1">
         <v>42643</v>
       </c>
-      <c r="U3" s="1" t="n">
+      <c r="U3" s="1">
         <v>42674</v>
       </c>
-      <c r="V3" s="1" t="n">
+      <c r="V3" s="1">
         <v>42704</v>
       </c>
-      <c r="W3" s="1" t="n">
+      <c r="W3" s="1">
         <v>42735</v>
       </c>
-      <c r="X3" s="1" t="n">
+      <c r="X3" s="1">
         <v>42766</v>
       </c>
-      <c r="Y3" s="1" t="n">
+      <c r="Y3" s="1">
         <v>42794</v>
       </c>
-      <c r="Z3" s="1" t="n">
+      <c r="Z3" s="1">
         <v>42825</v>
       </c>
-      <c r="AA3" s="1" t="n">
+      <c r="AA3" s="1">
         <v>42855</v>
       </c>
-      <c r="AB3" s="1" t="n">
+      <c r="AB3" s="1">
         <v>42886</v>
       </c>
-      <c r="AC3" s="1" t="n">
+      <c r="AC3" s="1">
         <v>42916</v>
       </c>
-      <c r="AD3" s="1" t="n">
+      <c r="AD3" s="1">
         <v>42947</v>
       </c>
-      <c r="AE3" s="1" t="n">
+      <c r="AE3" s="1">
         <v>42978</v>
       </c>
-      <c r="AF3" s="1" t="n">
+      <c r="AF3" s="1">
         <v>43008</v>
       </c>
-      <c r="AG3" s="1" t="n">
+      <c r="AG3" s="1">
         <v>43039</v>
       </c>
-      <c r="AH3" s="1" t="n">
+      <c r="AH3" s="1">
         <v>43069</v>
       </c>
-      <c r="AI3" s="1" t="n">
+      <c r="AI3" s="1">
         <v>43100</v>
       </c>
-      <c r="AJ3" s="1" t="n">
+      <c r="AJ3" s="1">
         <v>43131</v>
       </c>
-      <c r="AK3" s="1" t="n">
+      <c r="AK3" s="1">
         <v>43159</v>
       </c>
-      <c r="AL3" s="1" t="n">
+      <c r="AL3" s="1">
         <v>43190</v>
       </c>
-      <c r="AM3" s="1" t="n">
+      <c r="AM3" s="1">
         <v>43220</v>
       </c>
-      <c r="AN3" s="1" t="n">
+      <c r="AN3" s="1">
         <v>43251</v>
       </c>
-      <c r="AO3" s="1" t="n">
+      <c r="AO3" s="1">
         <v>43281</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
-      <c r="A4">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
         <f>Scenarios!A1</f>
-        <v/>
+        <v>annual_inflation</v>
       </c>
       <c r="C4">
         <f>Scenarios!C1</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="E4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="F4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="G4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="H4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="J4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="K4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="L4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="M4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="N4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="O4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="P4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Q4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="R4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="S4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="T4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="U4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="V4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="W4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="X4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Y4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Z4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AA4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AB4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AC4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AD4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AE4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AF4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AG4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AH4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AI4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AJ4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AK4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AL4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AM4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AN4">
         <f>C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AO4">
         <f>C4</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
-      <c r="A5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f>Scenarios!A2</f>
-        <v/>
+        <v>ltm ga</v>
       </c>
       <c r="C5">
         <f>Scenarios!C2</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="E5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="F5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="G5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="H5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="I5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="J5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="K5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="L5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="M5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="N5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="O5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="P5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Q5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="R5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="S5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="T5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="U5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="V5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="W5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="X5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Y5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Z5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AA5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AB5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AC5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AD5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AE5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AF5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AG5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AH5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AI5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AJ5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AK5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AL5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AM5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AN5">
         <f>C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AO5">
         <f>C5</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
-      <c r="A6">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>Scenarios!A3</f>
-        <v/>
+        <v>ltm marketing</v>
       </c>
       <c r="C6">
         <f>Scenarios!C3</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="E6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="F6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="G6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="H6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="I6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="J6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="K6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="L6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="M6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="N6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="O6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="P6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Q6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="R6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="S6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="T6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="U6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="V6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="W6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="X6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Y6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Z6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AA6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AB6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AC6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AD6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AE6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AF6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AG6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AH6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AI6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AJ6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AK6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AL6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AM6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AN6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AO6">
         <f>C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AO21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScale="80">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="D4" xSplit="3" ySplit="3"/>
+    <sheetView showGridLines="0" zoomScale="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="E3" s="1">
         <f>Timeline!E3</f>
-        <v/>
+        <v>42185</v>
       </c>
       <c r="F3" s="1">
         <f>Timeline!F3</f>
-        <v/>
+        <v>42216</v>
       </c>
       <c r="G3" s="1">
         <f>Timeline!G3</f>
-        <v/>
+        <v>42247</v>
       </c>
       <c r="H3" s="1">
         <f>Timeline!H3</f>
-        <v/>
+        <v>42277</v>
       </c>
       <c r="I3" s="1">
         <f>Timeline!I3</f>
-        <v/>
+        <v>42308</v>
       </c>
       <c r="J3" s="1">
         <f>Timeline!J3</f>
-        <v/>
+        <v>42338</v>
       </c>
       <c r="K3" s="1">
         <f>Timeline!K3</f>
-        <v/>
+        <v>42369</v>
       </c>
       <c r="L3" s="1">
         <f>Timeline!L3</f>
-        <v/>
+        <v>42400</v>
       </c>
       <c r="M3" s="1">
         <f>Timeline!M3</f>
-        <v/>
+        <v>42429</v>
       </c>
       <c r="N3" s="1">
         <f>Timeline!N3</f>
-        <v/>
+        <v>42460</v>
       </c>
       <c r="O3" s="1">
         <f>Timeline!O3</f>
-        <v/>
+        <v>42490</v>
       </c>
       <c r="P3" s="1">
         <f>Timeline!P3</f>
-        <v/>
+        <v>42521</v>
       </c>
       <c r="Q3" s="1">
         <f>Timeline!Q3</f>
-        <v/>
+        <v>42551</v>
       </c>
       <c r="R3" s="1">
         <f>Timeline!R3</f>
-        <v/>
+        <v>42582</v>
       </c>
       <c r="S3" s="1">
         <f>Timeline!S3</f>
-        <v/>
+        <v>42613</v>
       </c>
       <c r="T3" s="1">
         <f>Timeline!T3</f>
-        <v/>
+        <v>42643</v>
       </c>
       <c r="U3" s="1">
         <f>Timeline!U3</f>
-        <v/>
+        <v>42674</v>
       </c>
       <c r="V3" s="1">
         <f>Timeline!V3</f>
-        <v/>
+        <v>42704</v>
       </c>
       <c r="W3" s="1">
         <f>Timeline!W3</f>
-        <v/>
+        <v>42735</v>
       </c>
       <c r="X3" s="1">
         <f>Timeline!X3</f>
-        <v/>
+        <v>42766</v>
       </c>
       <c r="Y3" s="1">
         <f>Timeline!Y3</f>
-        <v/>
+        <v>42794</v>
       </c>
       <c r="Z3" s="1">
         <f>Timeline!Z3</f>
-        <v/>
+        <v>42825</v>
       </c>
       <c r="AA3" s="1">
         <f>Timeline!AA3</f>
-        <v/>
+        <v>42855</v>
       </c>
       <c r="AB3" s="1">
         <f>Timeline!AB3</f>
-        <v/>
+        <v>42886</v>
       </c>
       <c r="AC3" s="1">
         <f>Timeline!AC3</f>
-        <v/>
+        <v>42916</v>
       </c>
       <c r="AD3" s="1">
         <f>Timeline!AD3</f>
-        <v/>
+        <v>42947</v>
       </c>
       <c r="AE3" s="1">
         <f>Timeline!AE3</f>
-        <v/>
+        <v>42978</v>
       </c>
       <c r="AF3" s="1">
         <f>Timeline!AF3</f>
-        <v/>
+        <v>43008</v>
       </c>
       <c r="AG3" s="1">
         <f>Timeline!AG3</f>
-        <v/>
+        <v>43039</v>
       </c>
       <c r="AH3" s="1">
         <f>Timeline!AH3</f>
-        <v/>
+        <v>43069</v>
       </c>
       <c r="AI3" s="1">
         <f>Timeline!AI3</f>
-        <v/>
+        <v>43100</v>
       </c>
       <c r="AJ3" s="1">
         <f>Timeline!AJ3</f>
-        <v/>
+        <v>43131</v>
       </c>
       <c r="AK3" s="1">
         <f>Timeline!AK3</f>
-        <v/>
+        <v>43159</v>
       </c>
       <c r="AL3" s="1">
         <f>Timeline!AL3</f>
-        <v/>
+        <v>43190</v>
       </c>
       <c r="AM3" s="1">
         <f>Timeline!AM3</f>
-        <v/>
+        <v>43220</v>
       </c>
       <c r="AN3" s="1">
         <f>Timeline!AN3</f>
-        <v/>
+        <v>43251</v>
       </c>
       <c r="AO3" s="1">
         <f>Timeline!AO3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:41">
-      <c r="A4">
+        <v>43281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
         <f>Timeline!A4</f>
-        <v/>
+        <v>annual_inflation</v>
       </c>
       <c r="C4">
         <f>Timeline!C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="E4">
         <f>Timeline!E4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="F4">
         <f>Timeline!F4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="G4">
         <f>Timeline!G4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="H4">
         <f>Timeline!H4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <f>Timeline!I4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="J4">
         <f>Timeline!J4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="K4">
         <f>Timeline!K4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="L4">
         <f>Timeline!L4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="M4">
         <f>Timeline!M4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="N4">
         <f>Timeline!N4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="O4">
         <f>Timeline!O4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="P4">
         <f>Timeline!P4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Q4">
         <f>Timeline!Q4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="R4">
         <f>Timeline!R4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="S4">
         <f>Timeline!S4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="T4">
         <f>Timeline!T4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="U4">
         <f>Timeline!U4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="V4">
         <f>Timeline!V4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="W4">
         <f>Timeline!W4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="X4">
         <f>Timeline!X4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Y4">
         <f>Timeline!Y4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Z4">
         <f>Timeline!Z4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AA4">
         <f>Timeline!AA4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AB4">
         <f>Timeline!AB4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AC4">
         <f>Timeline!AC4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AD4">
         <f>Timeline!AD4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AE4">
         <f>Timeline!AE4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AF4">
         <f>Timeline!AF4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AG4">
         <f>Timeline!AG4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AH4">
         <f>Timeline!AH4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AI4">
         <f>Timeline!AI4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AJ4">
         <f>Timeline!AJ4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AK4">
         <f>Timeline!AK4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AL4">
         <f>Timeline!AL4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AM4">
         <f>Timeline!AM4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AN4">
         <f>Timeline!AN4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AO4">
         <f>Timeline!AO4</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
-      <c r="A5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f>Timeline!A5</f>
-        <v/>
+        <v>ltm ga</v>
       </c>
       <c r="C5">
         <f>Timeline!C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="E5">
         <f>Timeline!E5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="F5">
         <f>Timeline!F5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="G5">
         <f>Timeline!G5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="H5">
         <f>Timeline!H5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="I5">
         <f>Timeline!I5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="J5">
         <f>Timeline!J5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="K5">
         <f>Timeline!K5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="L5">
         <f>Timeline!L5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="M5">
         <f>Timeline!M5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="N5">
         <f>Timeline!N5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="O5">
         <f>Timeline!O5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="P5">
         <f>Timeline!P5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Q5">
         <f>Timeline!Q5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="R5">
         <f>Timeline!R5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="S5">
         <f>Timeline!S5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="T5">
         <f>Timeline!T5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="U5">
         <f>Timeline!U5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="V5">
         <f>Timeline!V5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="W5">
         <f>Timeline!W5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="X5">
         <f>Timeline!X5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Y5">
         <f>Timeline!Y5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Z5">
         <f>Timeline!Z5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AA5">
         <f>Timeline!AA5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AB5">
         <f>Timeline!AB5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AC5">
         <f>Timeline!AC5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AD5">
         <f>Timeline!AD5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AE5">
         <f>Timeline!AE5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AF5">
         <f>Timeline!AF5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AG5">
         <f>Timeline!AG5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AH5">
         <f>Timeline!AH5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AI5">
         <f>Timeline!AI5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AJ5">
         <f>Timeline!AJ5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AK5">
         <f>Timeline!AK5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AL5">
         <f>Timeline!AL5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AM5">
         <f>Timeline!AM5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AN5">
         <f>Timeline!AN5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AO5">
         <f>Timeline!AO5</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
-      <c r="A6">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>Timeline!A6</f>
-        <v/>
+        <v>ltm marketing</v>
       </c>
       <c r="C6">
         <f>Timeline!C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="E6">
         <f>Timeline!E6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="F6">
         <f>Timeline!F6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="G6">
         <f>Timeline!G6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="H6">
         <f>Timeline!H6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="I6">
         <f>Timeline!I6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="J6">
         <f>Timeline!J6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="K6">
         <f>Timeline!K6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="L6">
         <f>Timeline!L6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="M6">
         <f>Timeline!M6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="N6">
         <f>Timeline!N6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="O6">
         <f>Timeline!O6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="P6">
         <f>Timeline!P6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Q6">
         <f>Timeline!Q6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="R6">
         <f>Timeline!R6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="S6">
         <f>Timeline!S6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="T6">
         <f>Timeline!T6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="U6">
         <f>Timeline!U6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="V6">
         <f>Timeline!V6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="W6">
         <f>Timeline!W6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="X6">
         <f>Timeline!X6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Y6">
         <f>Timeline!Y6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Z6">
         <f>Timeline!Z6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AA6">
         <f>Timeline!AA6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AB6">
         <f>Timeline!AB6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AC6">
         <f>Timeline!AC6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AD6">
         <f>Timeline!AD6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AE6">
         <f>Timeline!AE6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AF6">
         <f>Timeline!AF6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AG6">
         <f>Timeline!AG6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AH6">
         <f>Timeline!AH6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AI6">
         <f>Timeline!AI6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AJ6">
         <f>Timeline!AJ6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AK6">
         <f>Timeline!AK6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AL6">
         <f>Timeline!AL6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AM6">
         <f>Timeline!AM6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AN6">
         <f>Timeline!AN6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AO6">
         <f>Timeline!AO6</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:41">
+        <v>453.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1">
         <f>E3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:41">
+        <v>42185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="E11">
         <f>IF(E18, E9-E18)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:41">
+        <v>6269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="b">
         <f>IF(AND(E18&lt;=E9,E9&lt;E21),TRUE,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="E13">
         <f>IF(E21, E21-E18)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:41">
+        <v>18250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="E14">
         <f>IF(E13, ROUND(E11/E13*100,0))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:41">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="1">
         <v>35551</v>
       </c>
       <c r="E17" s="1">
         <f>C17</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:41">
+        <v>35551</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="1">
         <v>35916</v>
       </c>
       <c r="E18" s="1">
         <f>C18</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:41">
+        <v>35916</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>41391</v>
       </c>
       <c r="E19" s="1">
         <f>C19</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:41">
+        <v>41391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="1">
         <v>48691</v>
       </c>
       <c r="E20" s="1">
         <f>C20</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:41">
+        <v>48691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="1">
         <v>54166</v>
       </c>
       <c r="E21" s="1">
         <f>C21</f>
-        <v/>
+        <v>54166</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AO70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0" zoomScale="80">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="D4" xSplit="3" ySplit="3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="E3" s="1">
         <f>Timeline!E3</f>
-        <v/>
+        <v>42185</v>
       </c>
       <c r="F3" s="1">
         <f>Timeline!F3</f>
-        <v/>
+        <v>42216</v>
       </c>
       <c r="G3" s="1">
         <f>Timeline!G3</f>
-        <v/>
+        <v>42247</v>
       </c>
       <c r="H3" s="1">
         <f>Timeline!H3</f>
-        <v/>
+        <v>42277</v>
       </c>
       <c r="I3" s="1">
         <f>Timeline!I3</f>
-        <v/>
+        <v>42308</v>
       </c>
       <c r="J3" s="1">
         <f>Timeline!J3</f>
-        <v/>
+        <v>42338</v>
       </c>
       <c r="K3" s="1">
         <f>Timeline!K3</f>
-        <v/>
+        <v>42369</v>
       </c>
       <c r="L3" s="1">
         <f>Timeline!L3</f>
-        <v/>
+        <v>42400</v>
       </c>
       <c r="M3" s="1">
         <f>Timeline!M3</f>
-        <v/>
+        <v>42429</v>
       </c>
       <c r="N3" s="1">
         <f>Timeline!N3</f>
-        <v/>
+        <v>42460</v>
       </c>
       <c r="O3" s="1">
         <f>Timeline!O3</f>
-        <v/>
+        <v>42490</v>
       </c>
       <c r="P3" s="1">
         <f>Timeline!P3</f>
-        <v/>
+        <v>42521</v>
       </c>
       <c r="Q3" s="1">
         <f>Timeline!Q3</f>
-        <v/>
+        <v>42551</v>
       </c>
       <c r="R3" s="1">
         <f>Timeline!R3</f>
-        <v/>
+        <v>42582</v>
       </c>
       <c r="S3" s="1">
         <f>Timeline!S3</f>
-        <v/>
+        <v>42613</v>
       </c>
       <c r="T3" s="1">
         <f>Timeline!T3</f>
-        <v/>
+        <v>42643</v>
       </c>
       <c r="U3" s="1">
         <f>Timeline!U3</f>
-        <v/>
+        <v>42674</v>
       </c>
       <c r="V3" s="1">
         <f>Timeline!V3</f>
-        <v/>
+        <v>42704</v>
       </c>
       <c r="W3" s="1">
         <f>Timeline!W3</f>
-        <v/>
+        <v>42735</v>
       </c>
       <c r="X3" s="1">
         <f>Timeline!X3</f>
-        <v/>
+        <v>42766</v>
       </c>
       <c r="Y3" s="1">
         <f>Timeline!Y3</f>
-        <v/>
+        <v>42794</v>
       </c>
       <c r="Z3" s="1">
         <f>Timeline!Z3</f>
-        <v/>
+        <v>42825</v>
       </c>
       <c r="AA3" s="1">
         <f>Timeline!AA3</f>
-        <v/>
+        <v>42855</v>
       </c>
       <c r="AB3" s="1">
         <f>Timeline!AB3</f>
-        <v/>
+        <v>42886</v>
       </c>
       <c r="AC3" s="1">
         <f>Timeline!AC3</f>
-        <v/>
+        <v>42916</v>
       </c>
       <c r="AD3" s="1">
         <f>Timeline!AD3</f>
-        <v/>
+        <v>42947</v>
       </c>
       <c r="AE3" s="1">
         <f>Timeline!AE3</f>
-        <v/>
+        <v>42978</v>
       </c>
       <c r="AF3" s="1">
         <f>Timeline!AF3</f>
-        <v/>
+        <v>43008</v>
       </c>
       <c r="AG3" s="1">
         <f>Timeline!AG3</f>
-        <v/>
+        <v>43039</v>
       </c>
       <c r="AH3" s="1">
         <f>Timeline!AH3</f>
-        <v/>
+        <v>43069</v>
       </c>
       <c r="AI3" s="1">
         <f>Timeline!AI3</f>
-        <v/>
+        <v>43100</v>
       </c>
       <c r="AJ3" s="1">
         <f>Timeline!AJ3</f>
-        <v/>
+        <v>43131</v>
       </c>
       <c r="AK3" s="1">
         <f>Timeline!AK3</f>
-        <v/>
+        <v>43159</v>
       </c>
       <c r="AL3" s="1">
         <f>Timeline!AL3</f>
-        <v/>
+        <v>43190</v>
       </c>
       <c r="AM3" s="1">
         <f>Timeline!AM3</f>
-        <v/>
+        <v>43220</v>
       </c>
       <c r="AN3" s="1">
         <f>Timeline!AN3</f>
-        <v/>
+        <v>43251</v>
       </c>
       <c r="AO3" s="1">
         <f>Timeline!AO3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:41">
-      <c r="A4">
+        <v>43281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
         <f>Timeline!A4</f>
-        <v/>
+        <v>annual_inflation</v>
       </c>
       <c r="C4">
         <f>Timeline!C4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="E4">
         <f>Timeline!E4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="F4">
         <f>Timeline!F4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="G4">
         <f>Timeline!G4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="H4">
         <f>Timeline!H4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="I4">
         <f>Timeline!I4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="J4">
         <f>Timeline!J4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="K4">
         <f>Timeline!K4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="L4">
         <f>Timeline!L4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="M4">
         <f>Timeline!M4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="N4">
         <f>Timeline!N4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="O4">
         <f>Timeline!O4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="P4">
         <f>Timeline!P4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Q4">
         <f>Timeline!Q4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="R4">
         <f>Timeline!R4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="S4">
         <f>Timeline!S4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="T4">
         <f>Timeline!T4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="U4">
         <f>Timeline!U4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="V4">
         <f>Timeline!V4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="W4">
         <f>Timeline!W4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="X4">
         <f>Timeline!X4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Y4">
         <f>Timeline!Y4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="Z4">
         <f>Timeline!Z4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AA4">
         <f>Timeline!AA4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AB4">
         <f>Timeline!AB4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AC4">
         <f>Timeline!AC4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AD4">
         <f>Timeline!AD4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AE4">
         <f>Timeline!AE4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AF4">
         <f>Timeline!AF4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AG4">
         <f>Timeline!AG4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AH4">
         <f>Timeline!AH4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AI4">
         <f>Timeline!AI4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AJ4">
         <f>Timeline!AJ4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AK4">
         <f>Timeline!AK4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AL4">
         <f>Timeline!AL4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AM4">
         <f>Timeline!AM4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AN4">
         <f>Timeline!AN4</f>
-        <v/>
+        <v>0.03</v>
       </c>
       <c r="AO4">
         <f>Timeline!AO4</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:41">
-      <c r="A5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
         <f>Timeline!A5</f>
-        <v/>
+        <v>ltm ga</v>
       </c>
       <c r="C5">
         <f>Timeline!C5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="E5">
         <f>Timeline!E5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="F5">
         <f>Timeline!F5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="G5">
         <f>Timeline!G5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="H5">
         <f>Timeline!H5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="I5">
         <f>Timeline!I5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="J5">
         <f>Timeline!J5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="K5">
         <f>Timeline!K5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="L5">
         <f>Timeline!L5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="M5">
         <f>Timeline!M5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="N5">
         <f>Timeline!N5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="O5">
         <f>Timeline!O5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="P5">
         <f>Timeline!P5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Q5">
         <f>Timeline!Q5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="R5">
         <f>Timeline!R5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="S5">
         <f>Timeline!S5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="T5">
         <f>Timeline!T5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="U5">
         <f>Timeline!U5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="V5">
         <f>Timeline!V5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="W5">
         <f>Timeline!W5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="X5">
         <f>Timeline!X5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Y5">
         <f>Timeline!Y5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="Z5">
         <f>Timeline!Z5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AA5">
         <f>Timeline!AA5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AB5">
         <f>Timeline!AB5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AC5">
         <f>Timeline!AC5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AD5">
         <f>Timeline!AD5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AE5">
         <f>Timeline!AE5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AF5">
         <f>Timeline!AF5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AG5">
         <f>Timeline!AG5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AH5">
         <f>Timeline!AH5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AI5">
         <f>Timeline!AI5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AJ5">
         <f>Timeline!AJ5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AK5">
         <f>Timeline!AK5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AL5">
         <f>Timeline!AL5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AM5">
         <f>Timeline!AM5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AN5">
         <f>Timeline!AN5</f>
-        <v/>
+        <v>8080</v>
       </c>
       <c r="AO5">
         <f>Timeline!AO5</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:41">
-      <c r="A6">
+        <v>8080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
         <f>Timeline!A6</f>
-        <v/>
+        <v>ltm marketing</v>
       </c>
       <c r="C6">
         <f>Timeline!C6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="E6">
         <f>Timeline!E6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="F6">
         <f>Timeline!F6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="G6">
         <f>Timeline!G6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="H6">
         <f>Timeline!H6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="I6">
         <f>Timeline!I6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="J6">
         <f>Timeline!J6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="K6">
         <f>Timeline!K6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="L6">
         <f>Timeline!L6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="M6">
         <f>Timeline!M6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="N6">
         <f>Timeline!N6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="O6">
         <f>Timeline!O6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="P6">
         <f>Timeline!P6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Q6">
         <f>Timeline!Q6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="R6">
         <f>Timeline!R6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="S6">
         <f>Timeline!S6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="T6">
         <f>Timeline!T6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="U6">
         <f>Timeline!U6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="V6">
         <f>Timeline!V6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="W6">
         <f>Timeline!W6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="X6">
         <f>Timeline!X6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Y6">
         <f>Timeline!Y6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="Z6">
         <f>Timeline!Z6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AA6">
         <f>Timeline!AA6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AB6">
         <f>Timeline!AB6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AC6">
         <f>Timeline!AC6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AD6">
         <f>Timeline!AD6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AE6">
         <f>Timeline!AE6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AF6">
         <f>Timeline!AF6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AG6">
         <f>Timeline!AG6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AH6">
         <f>Timeline!AH6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AI6">
         <f>Timeline!AI6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AJ6">
         <f>Timeline!AJ6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AK6">
         <f>Timeline!AK6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AL6">
         <f>Timeline!AL6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AM6">
         <f>Timeline!AM6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AN6">
         <f>Timeline!AN6</f>
-        <v/>
+        <v>453.2</v>
       </c>
       <c r="AO6">
         <f>Timeline!AO6</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:41">
+        <v>453.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1">
         <f>E3</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:41">
+        <v>42185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="E11">
         <f>IF(E18, E9-E18)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:41">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="b">
         <f>IF(AND(E18&lt;=E9,E9&lt;E21),TRUE,FALSE)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="E13">
         <f>IF(E21, E21-E18)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:41">
+        <v>5475</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="E14">
         <f>IF(E13, ROUND(E11/E13*100,0))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="n">
+      <c r="C17" s="1">
         <v>41517</v>
       </c>
       <c r="E17" s="1">
         <f>C17</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:41">
+        <v>41517</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="1">
         <v>41760</v>
       </c>
       <c r="E18" s="1">
         <f>C18</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:41">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>42855</v>
       </c>
       <c r="E19" s="1">
         <f>C19</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:41">
+        <v>42855</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="1">
         <v>44497</v>
       </c>
       <c r="E20" s="1">
         <f>C20</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:41">
+        <v>44497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="1" t="n">
+      <c r="C21" s="1">
         <v>47235</v>
       </c>
       <c r="E21" s="1">
         <f>C21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:41">
+        <v>47235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>1000000</v>
       </c>
     </row>
-    <row r="24" spans="1:41">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="E24">
         <f>E23/12*E14/(20-0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:41">
+        <v>33333.333333333328</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="E25">
         <f>E24</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:41">
+        <v>33333.333333333328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>0.65</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="E28">
         <f>IF(E12, 'existing 9'!E25 * (1-E27))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:41">
+        <v>11666.666666666664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
       <c r="E29">
         <f>E28</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:41">
+        <v>11666.666666666664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:41">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>20</v>
       </c>
-      <c r="E35" t="n">
+      <c r="E35">
         <v>2015</v>
       </c>
     </row>
-    <row r="36" spans="1:41">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
-      <c r="E36" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="37" spans="1:41">
+      <c r="E36">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
-      <c r="E37" t="n">
+      <c r="E37">
         <v>300000</v>
       </c>
     </row>
-    <row r="38" spans="1:41">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
       <c r="E38">
         <f>IF(E12,E37/12*(1+E36)^0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:41">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
       <c r="E39">
         <f>E38</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:41">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2790,41 +2913,41 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:41">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>2000</v>
       </c>
     </row>
-    <row r="43" spans="1:41">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
       <c r="E43">
         <f>E42*E12</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
       <c r="E44">
         <f>E43</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:41">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -2832,49 +2955,49 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:41">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>33</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>2000</v>
       </c>
     </row>
-    <row r="49" spans="1:41">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>34</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:41">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="E50">
         <f>MIN(+MAX(+'existing 9'!E44*E46, E49), E48)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
       <c r="E51">
         <f>E50</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>0.02</v>
       </c>
     </row>
-    <row r="56" spans="1:41">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2882,33 +3005,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:41">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>39</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:41">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>40</v>
       </c>
       <c r="E58">
         <f>MAX(+'existing 9'!E44*E55, E57)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>41</v>
       </c>
       <c r="E59">
         <f>E58</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>42</v>
       </c>
@@ -2916,74 +3039,76 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:41">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>44</v>
       </c>
-      <c r="E62" t="n">
+      <c r="E62">
         <v>500</v>
       </c>
     </row>
-    <row r="63" spans="1:41">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>45</v>
       </c>
       <c r="E63">
         <f>E62*E12</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>46</v>
       </c>
       <c r="E64">
         <f>E63</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>47</v>
       </c>
       <c r="E65">
         <f>'existing 9'!E59+'existing 9'!E64</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:41">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>48</v>
       </c>
       <c r="E66">
         <f>E65</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:41">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>49</v>
       </c>
       <c r="E67">
         <f>'existing 9'!E33+'existing 9'!E39+'existing 9'!E44+'existing 9'!E51+'existing 9'!E66</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:41">
+        <v>27700</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>50</v>
       </c>
       <c r="E68">
         <f>E67</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:41">
+        <v>27700</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>